<commit_message>
added template to add to worksheet 2
</commit_message>
<xml_diff>
--- a/django/django_project/geneData.xlsx
+++ b/django/django_project/geneData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>studyId</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>type of study</t>
+  </si>
+  <si>
+    <t>entryId</t>
   </si>
   <si>
     <t>27098879</t>
@@ -392,13 +395,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -408,12 +411,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add meta analysis and forest plot function
</commit_message>
<xml_diff>
--- a/django/django_project/geneData.xlsx
+++ b/django/django_project/geneData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>studyId</t>
   </si>
@@ -29,9 +29,153 @@
     <t>type of study</t>
   </si>
   <si>
+    <t>ascertainment</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>the_domain</t>
+  </si>
+  <si>
+    <t>num_SNPs</t>
+  </si>
+  <si>
+    <t>num_polys</t>
+  </si>
+  <si>
+    <t>DX</t>
+  </si>
+  <si>
+    <t>Case_N</t>
+  </si>
+  <si>
+    <t>Case_perc_fem</t>
+  </si>
+  <si>
+    <t>Case_age</t>
+  </si>
+  <si>
+    <t>Control_N</t>
+  </si>
+  <si>
+    <t>Control_perc_fem</t>
+  </si>
+  <si>
+    <t>Control_age</t>
+  </si>
+  <si>
+    <t>num_families</t>
+  </si>
+  <si>
+    <t>num_affected</t>
+  </si>
+  <si>
+    <t>num_generations</t>
+  </si>
+  <si>
+    <t>mean_score</t>
+  </si>
+  <si>
+    <t>SD_score</t>
+  </si>
+  <si>
+    <t>measure_used</t>
+  </si>
+  <si>
+    <t>disorder</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
     <t>entryId</t>
   </si>
   <si>
+    <t>SNP_id</t>
+  </si>
+  <si>
+    <t>Meta_p_value</t>
+  </si>
+  <si>
+    <t>SNP_chromosome_location</t>
+  </si>
+  <si>
+    <t>SNP_chromosome_band</t>
+  </si>
+  <si>
+    <t>SNP_position</t>
+  </si>
+  <si>
+    <t>SNP_version</t>
+  </si>
+  <si>
+    <t>odds_risk</t>
+  </si>
+  <si>
+    <t>odds_risk_lci</t>
+  </si>
+  <si>
+    <t>odds_risk_uci</t>
+  </si>
+  <si>
+    <t>ethnicity_1000_pop</t>
+  </si>
+  <si>
+    <t>REF_allele</t>
+  </si>
+  <si>
+    <t>ALT_allele</t>
+  </si>
+  <si>
+    <t>EFF_score</t>
+  </si>
+  <si>
+    <t>EFF_var</t>
+  </si>
+  <si>
+    <t>mtc_pvalue</t>
+  </si>
+  <si>
+    <t>SNP_risk</t>
+  </si>
+  <si>
+    <t>SNP_test</t>
+  </si>
+  <si>
+    <t>SNP_hyperlink</t>
+  </si>
+  <si>
+    <t>gene_name</t>
+  </si>
+  <si>
+    <t>gene_ensmbl_id</t>
+  </si>
+  <si>
+    <t>gene_chr</t>
+  </si>
+  <si>
+    <t>gene_band</t>
+  </si>
+  <si>
+    <t>gene_start</t>
+  </si>
+  <si>
+    <t>gene_end</t>
+  </si>
+  <si>
+    <t>gene_risk_status</t>
+  </si>
+  <si>
+    <t>gene_hyperlink</t>
+  </si>
+  <si>
     <t>27098879</t>
   </si>
   <si>
@@ -39,6 +183,66 @@
   </si>
   <si>
     <t>candidate</t>
+  </si>
+  <si>
+    <t>East Asian</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>4:-plex SNPscan</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>xas</t>
+  </si>
+  <si>
+    <t>cx1</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>high.com</t>
+  </si>
+  <si>
+    <t>KROK</t>
+  </si>
+  <si>
+    <t>4000000</t>
+  </si>
+  <si>
+    <t>African</t>
+  </si>
+  <si>
+    <t>mee</t>
+  </si>
+  <si>
+    <t>learning</t>
   </si>
 </sst>
 </file>
@@ -370,13 +574,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,19 +593,231 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2">
+        <v>195</v>
+      </c>
+      <c r="M2">
+        <v>36</v>
+      </c>
+      <c r="N2">
+        <v>10.99</v>
+      </c>
+      <c r="O2">
+        <v>196</v>
+      </c>
+      <c r="P2">
+        <v>38</v>
+      </c>
+      <c r="Q2">
+        <v>10.99</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3">
+        <v>195</v>
+      </c>
+      <c r="M3">
+        <v>36</v>
+      </c>
+      <c r="N3">
+        <v>10.99</v>
+      </c>
+      <c r="O3">
+        <v>196</v>
+      </c>
+      <c r="P3">
+        <v>38</v>
+      </c>
+      <c r="Q3">
+        <v>10.99</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -411,20 +827,268 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:28">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2">
+        <v>3.4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2">
+        <v>23</v>
+      </c>
+      <c r="O2">
+        <v>23</v>
+      </c>
+      <c r="P2">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>3.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3">
+        <v>23</v>
+      </c>
+      <c r="O3">
+        <v>23</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found maryams meta analysis R file, switched back to using it
</commit_message>
<xml_diff>
--- a/django/django_project/geneData.xlsx
+++ b/django/django_project/geneData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>studyId</t>
   </si>
@@ -203,46 +203,16 @@
     <t>ab</t>
   </si>
   <si>
-    <t>xas</t>
-  </si>
-  <si>
-    <t>cx1</t>
-  </si>
-  <si>
-    <t>X</t>
+    <t>Dyslexia</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>high.com</t>
-  </si>
-  <si>
-    <t>KROK</t>
-  </si>
-  <si>
-    <t>4000000</t>
-  </si>
-  <si>
-    <t>African</t>
-  </si>
-  <si>
-    <t>mee</t>
-  </si>
-  <si>
-    <t>learning</t>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>google.com</t>
   </si>
 </sst>
 </file>
@@ -574,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -731,92 +701,12 @@
         <v>61</v>
       </c>
       <c r="X2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="Y2" t="s">
         <v>61</v>
       </c>
       <c r="Z2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3">
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3">
-        <v>195</v>
-      </c>
-      <c r="M3">
-        <v>36</v>
-      </c>
-      <c r="N3">
-        <v>10.99</v>
-      </c>
-      <c r="O3">
-        <v>196</v>
-      </c>
-      <c r="P3">
-        <v>38</v>
-      </c>
-      <c r="Q3">
-        <v>10.99</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3" t="s">
-        <v>61</v>
-      </c>
-      <c r="X3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -827,7 +717,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -921,174 +811,88 @@
     </row>
     <row r="2" spans="1:28">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2">
-        <v>3.4</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s">
         <v>64</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" t="s">
         <v>65</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2">
-        <v>23</v>
-      </c>
-      <c r="O2">
-        <v>23</v>
-      </c>
-      <c r="P2">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2">
-        <v>3</v>
-      </c>
-      <c r="V2" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>10</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>70</v>
       </c>
       <c r="AB2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3">
-        <v>3.4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3">
-        <v>23</v>
-      </c>
-      <c r="O3">
-        <v>23</v>
-      </c>
-      <c r="P3">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>69</v>
-      </c>
-      <c r="R3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" t="s">
-        <v>71</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
-      <c r="V3" t="s">
-        <v>69</v>
-      </c>
-      <c r="W3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>10</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed index access of excel file
</commit_message>
<xml_diff>
--- a/django/django_project/geneData.xlsx
+++ b/django/django_project/geneData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>studyId</t>
   </si>
@@ -206,13 +206,46 @@
     <t>Dyslexia</t>
   </si>
   <si>
+    <t>xas</t>
+  </si>
+  <si>
+    <t>cx1</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>gene</t>
-  </si>
-  <si>
-    <t>google.com</t>
+    <t>white</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>high.com</t>
+  </si>
+  <si>
+    <t>KROK</t>
+  </si>
+  <si>
+    <t>4000000</t>
+  </si>
+  <si>
+    <t>African</t>
+  </si>
+  <si>
+    <t>mee</t>
+  </si>
+  <si>
+    <t>learning</t>
   </si>
 </sst>
 </file>
@@ -544,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -710,6 +743,86 @@
         <v>61</v>
       </c>
     </row>
+    <row r="3" spans="1:26">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3">
+        <v>195</v>
+      </c>
+      <c r="M3">
+        <v>36</v>
+      </c>
+      <c r="N3">
+        <v>10.99</v>
+      </c>
+      <c r="O3">
+        <v>196</v>
+      </c>
+      <c r="P3">
+        <v>38</v>
+      </c>
+      <c r="Q3">
+        <v>10.99</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -717,7 +830,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -811,88 +924,174 @@
     </row>
     <row r="2" spans="1:28">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="W2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Z2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="AA2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="AB2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>3.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3">
+        <v>23</v>
+      </c>
+      <c r="O3">
+        <v>23</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
+        <v>70</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to contact and methods
</commit_message>
<xml_diff>
--- a/django/django_project/geneData.xlsx
+++ b/django/django_project/geneData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>studyId</t>
   </si>
@@ -176,6 +176,9 @@
     <t>gene_hyperlink</t>
   </si>
   <si>
+    <t>study_id</t>
+  </si>
+  <si>
     <t>27098879</t>
   </si>
   <si>
@@ -203,27 +206,18 @@
     <t>ab</t>
   </si>
   <si>
-    <t>Dyslexia</t>
+    <t>xas</t>
+  </si>
+  <si>
+    <t>cx1</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>gene</t>
-  </si>
-  <si>
-    <t>google.com</t>
-  </si>
-  <si>
-    <t>xas</t>
-  </si>
-  <si>
-    <t>cx1</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
@@ -243,6 +237,18 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>4000000</t>
+  </si>
+  <si>
+    <t>African</t>
+  </si>
+  <si>
+    <t>mee</t>
+  </si>
+  <si>
+    <t>learning</t>
   </si>
 </sst>
 </file>
@@ -665,25 +671,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -692,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L2">
         <v>195</v>
@@ -728,42 +734,42 @@
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" t="s">
-        <v>61</v>
-      </c>
       <c r="Z2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I3">
         <v>18</v>
@@ -772,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L3">
         <v>195</v>
@@ -808,16 +814,16 @@
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" t="s">
         <v>62</v>
       </c>
-      <c r="Y3" t="s">
-        <v>61</v>
-      </c>
       <c r="Z3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -827,13 +833,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -918,114 +924,117 @@
       <c r="AB1" t="s">
         <v>23</v>
       </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="U2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="V2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="W2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Z2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="AA2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="AB2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>3.4</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1037,13 +1046,13 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" t="s">
         <v>69</v>
-      </c>
-      <c r="L3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" t="s">
-        <v>71</v>
       </c>
       <c r="N3">
         <v>23</v>
@@ -1055,25 +1064,25 @@
         <v>23</v>
       </c>
       <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" t="s">
         <v>72</v>
       </c>
-      <c r="R3" t="s">
-        <v>72</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>73</v>
       </c>
-      <c r="T3" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" t="s">
-        <v>75</v>
-      </c>
       <c r="V3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="W3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -1082,13 +1091,13 @@
         <v>10</v>
       </c>
       <c r="Z3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AB3" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>